<commit_message>
po grid tax fetch bind
</commit_message>
<xml_diff>
--- a/MMGPA/Portal/Reference/Tendor_BOM.xlsx
+++ b/MMGPA/Portal/Reference/Tendor_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>ItemCategory</t>
   </si>
@@ -101,10 +101,7 @@
     <t>screws for machine repair</t>
   </si>
   <si>
-    <t>ReqBalanceQty</t>
-  </si>
-  <si>
-    <t>TendorQuantity</t>
+    <t>TenderQuantity</t>
   </si>
 </sst>
 </file>
@@ -460,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,14 +468,13 @@
     <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -492,24 +488,21 @@
         <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -522,20 +515,17 @@
       <c r="D3" s="1">
         <v>150</v>
       </c>
-      <c r="E3" s="1">
-        <v>150</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1">
+      <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -548,20 +538,17 @@
       <c r="D4" s="1">
         <v>200</v>
       </c>
-      <c r="E4" s="1">
-        <v>200</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1">
+      <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -574,20 +561,17 @@
       <c r="D5" s="1">
         <v>20</v>
       </c>
-      <c r="E5" s="1">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1">
+      <c r="F5" s="1">
         <v>3000</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -600,20 +584,17 @@
       <c r="D6" s="1">
         <v>30</v>
       </c>
-      <c r="E6" s="1">
-        <v>30</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1">
+      <c r="F6" s="1">
         <v>1500</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -626,16 +607,13 @@
       <c r="D7" s="1">
         <v>60</v>
       </c>
-      <c r="E7" s="1">
-        <v>60</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1">
+      <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>